<commit_message>
Layout changes / Rode Diesel pagina
</commit_message>
<xml_diff>
--- a/Uren Grenspoal - Dominic.xlsx
+++ b/Uren Grenspoal - Dominic.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Datum</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Aanpassen lay-out</t>
+  </si>
+  <si>
+    <t>Layout</t>
   </si>
 </sst>
 </file>
@@ -391,7 +394,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,8 +430,8 @@
         <v>5</v>
       </c>
       <c r="D2" s="2">
-        <f>SUM(B2:B30)</f>
-        <v>14</v>
+        <f>SUM(B2:B8)</f>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -492,9 +495,15 @@
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="A8" s="1">
+        <v>42381</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update layout/ Rode Diesel pagina / uren
</commit_message>
<xml_diff>
--- a/Uren Grenspoal - Dominic.xlsx
+++ b/Uren Grenspoal - Dominic.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Datum</t>
   </si>
@@ -53,7 +53,10 @@
     <t>Aanpassen lay-out</t>
   </si>
   <si>
-    <t>Layout</t>
+    <t>Layout / Rode diesel pagina</t>
+  </si>
+  <si>
+    <t>Layout / Rode diesel pagina / Website tijdelijk online zetten</t>
   </si>
 </sst>
 </file>
@@ -394,7 +397,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,8 +433,8 @@
         <v>5</v>
       </c>
       <c r="D2" s="2">
-        <f>SUM(B2:B8)</f>
-        <v>16</v>
+        <f>SUM(B2:B9)</f>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -507,9 +510,15 @@
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="1">
+        <v>42029</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>